<commit_message>
premium HQ tp fix
</commit_message>
<xml_diff>
--- a/gu_in/Item.edf/22_TownItem/TOWNItem.xlsx
+++ b/gu_in/Item.edf/22_TownItem/TOWNItem.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8C9D5A-425F-49F5-A48C-CCFD0D98B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B381167E-7B51-404B-9EAA-241D571E6CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWNItem" sheetId="1" r:id="rId1"/>
@@ -1163,9 +1163,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1203,9 +1203,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1238,9 +1238,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1273,9 +1290,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1451,47 +1485,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J61" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V84" sqref="V84"/>
+      <selection pane="bottomRight" activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1580,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1667,7 +1701,7 @@
       </c>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1755,7 +1789,7 @@
       </c>
       <c r="AC3" s="2"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1843,7 +1877,7 @@
       </c>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1931,7 +1965,7 @@
       </c>
       <c r="AC5" s="2"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -2019,7 +2053,7 @@
       </c>
       <c r="AC6" s="2"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -2107,7 +2141,7 @@
       </c>
       <c r="AC7" s="2"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -2195,7 +2229,7 @@
       </c>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -2283,7 +2317,7 @@
       </c>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -2371,7 +2405,7 @@
       </c>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -2459,7 +2493,7 @@
       </c>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2547,7 +2581,7 @@
       </c>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -2635,7 +2669,7 @@
       </c>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
@@ -2723,7 +2757,7 @@
       </c>
       <c r="AC14" s="2"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>63</v>
       </c>
@@ -2811,7 +2845,7 @@
       </c>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>66</v>
       </c>
@@ -2899,7 +2933,7 @@
       </c>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>69</v>
       </c>
@@ -2987,7 +3021,7 @@
       </c>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>72</v>
       </c>
@@ -3075,7 +3109,7 @@
       </c>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -3163,7 +3197,7 @@
       </c>
       <c r="AC19" s="2"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -3251,7 +3285,7 @@
       </c>
       <c r="AC20" s="2"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>81</v>
       </c>
@@ -3339,7 +3373,7 @@
       </c>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -3427,7 +3461,7 @@
       </c>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>86</v>
       </c>
@@ -3515,7 +3549,7 @@
       </c>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>88</v>
       </c>
@@ -3603,7 +3637,7 @@
       </c>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>90</v>
       </c>
@@ -3691,7 +3725,7 @@
       </c>
       <c r="AC25" s="2"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>92</v>
       </c>
@@ -3779,7 +3813,7 @@
       </c>
       <c r="AC26" s="2"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>94</v>
       </c>
@@ -3867,7 +3901,7 @@
       </c>
       <c r="AC27" s="2"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>96</v>
       </c>
@@ -3955,7 +3989,7 @@
       </c>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>98</v>
       </c>
@@ -4043,7 +4077,7 @@
       </c>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>100</v>
       </c>
@@ -4131,7 +4165,7 @@
       </c>
       <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>102</v>
       </c>
@@ -4219,7 +4253,7 @@
       </c>
       <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>104</v>
       </c>
@@ -4307,7 +4341,7 @@
       </c>
       <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>106</v>
       </c>
@@ -4395,7 +4429,7 @@
       </c>
       <c r="AC33" s="2"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>108</v>
       </c>
@@ -4483,7 +4517,7 @@
       </c>
       <c r="AC34" s="2"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>110</v>
       </c>
@@ -4571,7 +4605,7 @@
       </c>
       <c r="AC35" s="2"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>112</v>
       </c>
@@ -4659,7 +4693,7 @@
       </c>
       <c r="AC36" s="2"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -4747,7 +4781,7 @@
       </c>
       <c r="AC37" s="2"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>116</v>
       </c>
@@ -4835,7 +4869,7 @@
       </c>
       <c r="AC38" s="2"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>118</v>
       </c>
@@ -4923,7 +4957,7 @@
       </c>
       <c r="AC39" s="2"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>120</v>
       </c>
@@ -5011,7 +5045,7 @@
       </c>
       <c r="AC40" s="2"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>122</v>
       </c>
@@ -5099,7 +5133,7 @@
       </c>
       <c r="AC41" s="2"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>124</v>
       </c>
@@ -5187,7 +5221,7 @@
       </c>
       <c r="AC42" s="2"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>126</v>
       </c>
@@ -5275,7 +5309,7 @@
       </c>
       <c r="AC43" s="2"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>128</v>
       </c>
@@ -5363,7 +5397,7 @@
       </c>
       <c r="AC44" s="2"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>130</v>
       </c>
@@ -5451,7 +5485,7 @@
       </c>
       <c r="AC45" s="2"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>132</v>
       </c>
@@ -5539,7 +5573,7 @@
       </c>
       <c r="AC46" s="2"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>134</v>
       </c>
@@ -5627,7 +5661,7 @@
       </c>
       <c r="AC47" s="2"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>136</v>
       </c>
@@ -5715,7 +5749,7 @@
       </c>
       <c r="AC48" s="2"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>138</v>
       </c>
@@ -5803,7 +5837,7 @@
       </c>
       <c r="AC49" s="2"/>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>140</v>
       </c>
@@ -5891,7 +5925,7 @@
       </c>
       <c r="AC50" s="2"/>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>142</v>
       </c>
@@ -5979,7 +6013,7 @@
       </c>
       <c r="AC51" s="2"/>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>144</v>
       </c>
@@ -6067,7 +6101,7 @@
       </c>
       <c r="AC52" s="2"/>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>146</v>
       </c>
@@ -6155,7 +6189,7 @@
       </c>
       <c r="AC53" s="2"/>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>148</v>
       </c>
@@ -6243,7 +6277,7 @@
       </c>
       <c r="AC54" s="2"/>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>150</v>
       </c>
@@ -6331,7 +6365,7 @@
       </c>
       <c r="AC55" s="2"/>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>152</v>
       </c>
@@ -6419,7 +6453,7 @@
       </c>
       <c r="AC56" s="2"/>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>153</v>
       </c>
@@ -6507,7 +6541,7 @@
       </c>
       <c r="AC57" s="2"/>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>155</v>
       </c>
@@ -6595,7 +6629,7 @@
       </c>
       <c r="AC58" s="2"/>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>156</v>
       </c>
@@ -6683,7 +6717,7 @@
       </c>
       <c r="AC59" s="2"/>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>158</v>
       </c>
@@ -6771,7 +6805,7 @@
       </c>
       <c r="AC60" s="2"/>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>160</v>
       </c>
@@ -6859,7 +6893,7 @@
       </c>
       <c r="AC61" s="2"/>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>162</v>
       </c>
@@ -6947,7 +6981,7 @@
       </c>
       <c r="AC62" s="2"/>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>165</v>
       </c>
@@ -7035,7 +7069,7 @@
       </c>
       <c r="AC63" s="2"/>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>167</v>
       </c>
@@ -7123,7 +7157,7 @@
       </c>
       <c r="AC64" s="2"/>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>169</v>
       </c>
@@ -7211,7 +7245,7 @@
       </c>
       <c r="AC65" s="2"/>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>170</v>
       </c>
@@ -7299,7 +7333,7 @@
       </c>
       <c r="AC66" s="2"/>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>172</v>
       </c>
@@ -7387,7 +7421,7 @@
       </c>
       <c r="AC67" s="2"/>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>174</v>
       </c>
@@ -7475,7 +7509,7 @@
       </c>
       <c r="AC68" s="2"/>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>176</v>
       </c>
@@ -7563,7 +7597,7 @@
       </c>
       <c r="AC69" s="2"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>178</v>
       </c>
@@ -7651,7 +7685,7 @@
       </c>
       <c r="AC70" s="2"/>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>180</v>
       </c>
@@ -7739,7 +7773,7 @@
       </c>
       <c r="AC71" s="2"/>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>182</v>
       </c>
@@ -7827,7 +7861,7 @@
       </c>
       <c r="AC72" s="2"/>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>184</v>
       </c>
@@ -7915,7 +7949,7 @@
       </c>
       <c r="AC73" s="2"/>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>187</v>
       </c>
@@ -8003,7 +8037,7 @@
       </c>
       <c r="AC74" s="2"/>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>190</v>
       </c>
@@ -8091,7 +8125,7 @@
       </c>
       <c r="AC75" s="2"/>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>191</v>
       </c>
@@ -8179,7 +8213,7 @@
       </c>
       <c r="AC76" s="2"/>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>193</v>
       </c>
@@ -8267,7 +8301,7 @@
       </c>
       <c r="AC77" s="2"/>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>196</v>
       </c>
@@ -8302,7 +8336,7 @@
         <v>0</v>
       </c>
       <c r="L78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78" s="3">
         <v>0</v>
@@ -8326,7 +8360,7 @@
         <v>-1</v>
       </c>
       <c r="T78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78" s="3">
         <v>0</v>
@@ -8335,7 +8369,7 @@
         <v>0</v>
       </c>
       <c r="W78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X78" s="2">
         <v>1</v>
@@ -8345,7 +8379,7 @@
         <v>tiqbpc01</v>
       </c>
       <c r="Z78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA78" s="3">
         <v>0</v>
@@ -8355,7 +8389,7 @@
       </c>
       <c r="AC78" s="2"/>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>197</v>
       </c>
@@ -8390,7 +8424,7 @@
         <v>0</v>
       </c>
       <c r="L79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" s="3">
         <v>0</v>
@@ -8414,7 +8448,7 @@
         <v>-1</v>
       </c>
       <c r="T79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U79" s="3">
         <v>0</v>
@@ -8423,7 +8457,7 @@
         <v>0</v>
       </c>
       <c r="W79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X79" s="2">
         <v>1</v>
@@ -8433,7 +8467,7 @@
         <v>tiqcpc01</v>
       </c>
       <c r="Z79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA79" s="3">
         <v>0</v>
@@ -8443,7 +8477,7 @@
       </c>
       <c r="AC79" s="2"/>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>198</v>
       </c>
@@ -8478,7 +8512,7 @@
         <v>0</v>
       </c>
       <c r="L80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M80" s="3">
         <v>0</v>
@@ -8502,7 +8536,7 @@
         <v>-1</v>
       </c>
       <c r="T80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U80" s="3">
         <v>0</v>
@@ -8511,7 +8545,7 @@
         <v>0</v>
       </c>
       <c r="W80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X80" s="2">
         <v>1</v>
@@ -8521,7 +8555,7 @@
         <v>tiqapc01</v>
       </c>
       <c r="Z80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA80" s="3">
         <v>0</v>
@@ -8531,7 +8565,7 @@
       </c>
       <c r="AC80" s="2"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>303</v>
       </c>
@@ -8618,7 +8652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>306</v>
       </c>
@@ -8705,7 +8739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>309</v>
       </c>
@@ -8792,7 +8826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>311</v>
       </c>
@@ -8879,7 +8913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>313</v>
       </c>
@@ -8966,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>316</v>
       </c>
@@ -9053,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>318</v>
       </c>
@@ -9140,7 +9174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>320</v>
       </c>
@@ -9227,7 +9261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>322</v>
       </c>
@@ -9314,7 +9348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>324</v>
       </c>
@@ -9411,46 +9445,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J70" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="X87" sqref="X87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>199</v>
       </c>
@@ -9539,7 +9573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>TOWNItem!A2</f>
         <v>Code</v>
@@ -9649,7 +9683,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>TOWNItem!A3</f>
         <v>iqbbb00</v>
@@ -9759,7 +9793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>TOWNItem!A4</f>
         <v>iqccc00</v>
@@ -9869,7 +9903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>TOWNItem!A5</f>
         <v>iqaaa00</v>
@@ -9979,7 +10013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>TOWNItem!A6</f>
         <v>iqbbb01</v>
@@ -10089,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>TOWNItem!A7</f>
         <v>iqccc01</v>
@@ -10199,7 +10233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>TOWNItem!A8</f>
         <v>iqaaa01</v>
@@ -10309,7 +10343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>TOWNItem!A9</f>
         <v>iqbbb02</v>
@@ -10419,7 +10453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>TOWNItem!A10</f>
         <v>iqccc02</v>
@@ -10529,7 +10563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>TOWNItem!A11</f>
         <v>iqaaa02</v>
@@ -10639,7 +10673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>TOWNItem!A12</f>
         <v>iqbnn01</v>
@@ -10749,7 +10783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>TOWNItem!A13</f>
         <v>iqbnn02</v>
@@ -10859,7 +10893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>TOWNItem!A14</f>
         <v>iqcnn01</v>
@@ -10969,7 +11003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>TOWNItem!A15</f>
         <v>iqcnn02</v>
@@ -11079,7 +11113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>TOWNItem!A16</f>
         <v>iqann01</v>
@@ -11189,7 +11223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>TOWNItem!A17</f>
         <v>iqann02</v>
@@ -11299,7 +11333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>TOWNItem!A18</f>
         <v>iqres01</v>
@@ -11409,7 +11443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>TOWNItem!A19</f>
         <v>iqell01</v>
@@ -11519,7 +11553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>TOWNItem!A20</f>
         <v>iqtwe01</v>
@@ -11629,7 +11663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>TOWNItem!A21</f>
         <v>iqcsa01</v>
@@ -11739,7 +11773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>TOWNItem!A22</f>
         <v>iqcsa02</v>
@@ -11849,7 +11883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>TOWNItem!A23</f>
         <v>iqcsa03</v>
@@ -11959,7 +11993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>TOWNItem!A24</f>
         <v>iqcsa04</v>
@@ -12069,7 +12103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>TOWNItem!A25</f>
         <v>iqcsa05</v>
@@ -12179,7 +12213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>TOWNItem!A26</f>
         <v>iqcsa06</v>
@@ -12289,7 +12323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>TOWNItem!A27</f>
         <v>iqcsa07</v>
@@ -12399,7 +12433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>TOWNItem!A28</f>
         <v>iqcsa08</v>
@@ -12509,7 +12543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>TOWNItem!A29</f>
         <v>iqcsa09</v>
@@ -12619,7 +12653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>TOWNItem!A30</f>
         <v>iqcsa10</v>
@@ -12729,7 +12763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>TOWNItem!A31</f>
         <v>iqcsa11</v>
@@ -12839,7 +12873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>TOWNItem!A32</f>
         <v>iqcsa12</v>
@@ -12949,7 +12983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>TOWNItem!A33</f>
         <v>iqcsa13</v>
@@ -13059,7 +13093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>TOWNItem!A34</f>
         <v>iqcsa14</v>
@@ -13169,7 +13203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>TOWNItem!A35</f>
         <v>iqcsa15</v>
@@ -13279,7 +13313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>TOWNItem!A36</f>
         <v>iqcsa16</v>
@@ -13389,7 +13423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>TOWNItem!A37</f>
         <v>iqcsa17</v>
@@ -13499,7 +13533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>TOWNItem!A38</f>
         <v>iqcsa18</v>
@@ -13609,7 +13643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>TOWNItem!A39</f>
         <v>iqcsa19</v>
@@ -13719,7 +13753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>TOWNItem!A40</f>
         <v>iqcsa20</v>
@@ -13829,7 +13863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>TOWNItem!A41</f>
         <v>iqcsa21</v>
@@ -13939,7 +13973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>TOWNItem!A42</f>
         <v>iqcsa22</v>
@@ -14049,7 +14083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>TOWNItem!A43</f>
         <v>iqcsa23</v>
@@ -14159,7 +14193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>TOWNItem!A44</f>
         <v>iqcsa24</v>
@@ -14269,7 +14303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>TOWNItem!A45</f>
         <v>iqcsa25</v>
@@ -14379,7 +14413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>TOWNItem!A46</f>
         <v>iqcsa26</v>
@@ -14489,7 +14523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>TOWNItem!A47</f>
         <v>iqcsa27</v>
@@ -14599,7 +14633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>TOWNItem!A48</f>
         <v>iqcsa28</v>
@@ -14709,7 +14743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>TOWNItem!A49</f>
         <v>iqcsa29</v>
@@ -14819,7 +14853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>TOWNItem!A50</f>
         <v>iqcsa30</v>
@@ -14929,7 +14963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>TOWNItem!A51</f>
         <v>iqcsa31</v>
@@ -15039,7 +15073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>TOWNItem!A52</f>
         <v>iqcsa32</v>
@@ -15149,7 +15183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>TOWNItem!A53</f>
         <v>iqcsa33</v>
@@ -15259,7 +15293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>TOWNItem!A54</f>
         <v>iqcsa34</v>
@@ -15369,7 +15403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>TOWNItem!A55</f>
         <v>iqcsa35</v>
@@ -15479,7 +15513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>TOWNItem!A56</f>
         <v>iqcsa36</v>
@@ -15589,7 +15623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>TOWNItem!A57</f>
         <v>iqcsa37</v>
@@ -15699,7 +15733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>TOWNItem!A58</f>
         <v>iqcsa38</v>
@@ -15809,7 +15843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>TOWNItem!A59</f>
         <v>iqcsa39</v>
@@ -15919,7 +15953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>TOWNItem!A60</f>
         <v>iqcsa40</v>
@@ -16029,7 +16063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>TOWNItem!A61</f>
         <v>iqcsa41</v>
@@ -16139,7 +16173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>TOWNItem!A62</f>
         <v>iqcsa42</v>
@@ -16249,7 +16283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>TOWNItem!A63</f>
         <v>iqcsa43</v>
@@ -16359,7 +16393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>TOWNItem!A64</f>
         <v>iqcsa44</v>
@@ -16469,7 +16503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>TOWNItem!A65</f>
         <v>iqcsa45</v>
@@ -16579,7 +16613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>TOWNItem!A66</f>
         <v>iqcsa46</v>
@@ -16689,7 +16723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>TOWNItem!A67</f>
         <v>iqcsa47</v>
@@ -16799,7 +16833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>TOWNItem!A68</f>
         <v>iqcsa48</v>
@@ -16909,7 +16943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>TOWNItem!A69</f>
         <v>iqcsa49</v>
@@ -17019,7 +17053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>TOWNItem!A70</f>
         <v>iqcsa50</v>
@@ -17129,7 +17163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>TOWNItem!A71</f>
         <v>iqcsa51</v>
@@ -17239,7 +17273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>TOWNItem!A72</f>
         <v>iqcsa52</v>
@@ -17349,7 +17383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>TOWNItem!A73</f>
         <v>iqcsa53</v>
@@ -17459,7 +17493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>TOWNItem!A74</f>
         <v>iqcsa54</v>
@@ -17569,7 +17603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>TOWNItem!A75</f>
         <v>iqcsa55</v>
@@ -17679,7 +17713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>TOWNItem!A76</f>
         <v>iqcsa56</v>
@@ -17789,7 +17823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>TOWNItem!A77</f>
         <v>iqcsa57</v>
@@ -17899,7 +17933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>TOWNItem!A78</f>
         <v>iqbpc01</v>
@@ -17932,7 +17966,7 @@
       </c>
       <c r="I78">
         <f>TOWNItem!L78</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78">
         <f>TOWNItem!M78</f>
@@ -17960,7 +17994,7 @@
       </c>
       <c r="P78">
         <f>TOWNItem!T78</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78">
         <f>TOWNItem!V78</f>
@@ -17968,7 +18002,7 @@
       </c>
       <c r="R78">
         <f>TOWNItem!W78</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S78" s="4">
         <v>75</v>
@@ -17979,7 +18013,7 @@
       </c>
       <c r="U78">
         <f>TOWNItem!Z78</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V78">
         <f>TOWNItem!AB78</f>
@@ -18009,7 +18043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>TOWNItem!A79</f>
         <v>iqcpc01</v>
@@ -18042,7 +18076,7 @@
       </c>
       <c r="I79">
         <f>TOWNItem!L79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79">
         <f>TOWNItem!M79</f>
@@ -18070,7 +18104,7 @@
       </c>
       <c r="P79">
         <f>TOWNItem!T79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q79">
         <f>TOWNItem!V79</f>
@@ -18078,7 +18112,7 @@
       </c>
       <c r="R79">
         <f>TOWNItem!W79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S79" s="4">
         <v>76</v>
@@ -18089,7 +18123,7 @@
       </c>
       <c r="U79">
         <f>TOWNItem!Z79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V79">
         <f>TOWNItem!AB79</f>
@@ -18119,7 +18153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>TOWNItem!A80</f>
         <v>iqapc01</v>
@@ -18152,7 +18186,7 @@
       </c>
       <c r="I80">
         <f>TOWNItem!L80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80">
         <f>TOWNItem!M80</f>
@@ -18180,7 +18214,7 @@
       </c>
       <c r="P80">
         <f>TOWNItem!T80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q80">
         <f>TOWNItem!V80</f>
@@ -18188,7 +18222,7 @@
       </c>
       <c r="R80">
         <f>TOWNItem!W80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S80" s="4">
         <v>77</v>
@@ -18199,7 +18233,7 @@
       </c>
       <c r="U80">
         <f>TOWNItem!Z80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V80">
         <f>TOWNItem!AB80</f>
@@ -18229,7 +18263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>TOWNItem!A81</f>
         <v>iqjet01</v>
@@ -18339,7 +18373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>TOWNItem!A82</f>
         <v>iqtow01</v>
@@ -18449,7 +18483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>TOWNItem!A83</f>
         <v>iqlic01</v>
@@ -18559,7 +18593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>TOWNItem!A84</f>
         <v>iqmus01</v>
@@ -18669,7 +18703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>TOWNItem!A85</f>
         <v>iqwou01</v>
@@ -18779,7 +18813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>TOWNItem!A86</f>
         <v>iqwou02</v>
@@ -18889,7 +18923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>TOWNItem!A87</f>
         <v>iqwou03</v>
@@ -18999,7 +19033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>TOWNItem!A88</f>
         <v>iqwou04</v>
@@ -19109,7 +19143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>TOWNItem!A89</f>
         <v>iqwou05</v>
@@ -19219,7 +19253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>TOWNItem!A90</f>
         <v>iqfei01</v>
@@ -19344,9 +19378,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -19357,7 +19391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>205</v>
       </c>
@@ -19366,7 +19400,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -19375,7 +19409,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -19384,7 +19418,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -19393,7 +19427,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -19402,7 +19436,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -19411,7 +19445,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -19420,7 +19454,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -19429,7 +19463,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -19438,7 +19472,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -19447,7 +19481,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -19456,7 +19490,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -19465,7 +19499,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -19474,7 +19508,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -19483,7 +19517,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -19492,7 +19526,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -19501,7 +19535,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -19510,7 +19544,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -19519,7 +19553,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -19528,7 +19562,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -19537,7 +19571,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -19546,7 +19580,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -19555,7 +19589,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -19564,7 +19598,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -19573,7 +19607,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -19582,7 +19616,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>24</v>
       </c>
@@ -19591,7 +19625,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -19600,7 +19634,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -19609,7 +19643,7 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -19618,7 +19652,7 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>28</v>
       </c>
@@ -19627,7 +19661,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>29</v>
       </c>
@@ -19636,7 +19670,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>30</v>
       </c>
@@ -19645,7 +19679,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -19654,7 +19688,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>32</v>
       </c>
@@ -19663,7 +19697,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>33</v>
       </c>
@@ -19672,7 +19706,7 @@
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>34</v>
       </c>
@@ -19681,7 +19715,7 @@
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -19690,7 +19724,7 @@
       </c>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>36</v>
       </c>
@@ -19699,7 +19733,7 @@
       </c>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -19708,7 +19742,7 @@
       </c>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>38</v>
       </c>
@@ -19717,7 +19751,7 @@
       </c>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39</v>
       </c>
@@ -19726,7 +19760,7 @@
       </c>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>40</v>
       </c>
@@ -19735,7 +19769,7 @@
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>41</v>
       </c>
@@ -19744,7 +19778,7 @@
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>42</v>
       </c>
@@ -19753,7 +19787,7 @@
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43</v>
       </c>
@@ -19762,7 +19796,7 @@
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44</v>
       </c>
@@ -19771,7 +19805,7 @@
       </c>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45</v>
       </c>
@@ -19780,7 +19814,7 @@
       </c>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>46</v>
       </c>
@@ -19789,7 +19823,7 @@
       </c>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -19798,7 +19832,7 @@
       </c>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>48</v>
       </c>
@@ -19807,7 +19841,7 @@
       </c>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>49</v>
       </c>
@@ -19816,7 +19850,7 @@
       </c>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>50</v>
       </c>
@@ -19825,7 +19859,7 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>51</v>
       </c>
@@ -19834,7 +19868,7 @@
       </c>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>52</v>
       </c>
@@ -19843,7 +19877,7 @@
       </c>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>53</v>
       </c>
@@ -19852,7 +19886,7 @@
       </c>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>54</v>
       </c>
@@ -19861,7 +19895,7 @@
       </c>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>55</v>
       </c>
@@ -19870,7 +19904,7 @@
       </c>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>56</v>
       </c>
@@ -19879,7 +19913,7 @@
       </c>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>57</v>
       </c>
@@ -19888,7 +19922,7 @@
       </c>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>58</v>
       </c>
@@ -19897,7 +19931,7 @@
       </c>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>59</v>
       </c>
@@ -19906,7 +19940,7 @@
       </c>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>60</v>
       </c>
@@ -19915,7 +19949,7 @@
       </c>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>61</v>
       </c>
@@ -19924,7 +19958,7 @@
       </c>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>62</v>
       </c>
@@ -19933,7 +19967,7 @@
       </c>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>63</v>
       </c>
@@ -19942,7 +19976,7 @@
       </c>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>64</v>
       </c>
@@ -19951,7 +19985,7 @@
       </c>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>65</v>
       </c>
@@ -19960,7 +19994,7 @@
       </c>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>66</v>
       </c>
@@ -19969,7 +20003,7 @@
       </c>
       <c r="C69" s="2"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>67</v>
       </c>
@@ -19978,7 +20012,7 @@
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>68</v>
       </c>
@@ -19987,7 +20021,7 @@
       </c>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>69</v>
       </c>
@@ -19996,7 +20030,7 @@
       </c>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>70</v>
       </c>
@@ -20005,7 +20039,7 @@
       </c>
       <c r="C73" s="2"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>71</v>
       </c>
@@ -20014,7 +20048,7 @@
       </c>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>72</v>
       </c>
@@ -20023,7 +20057,7 @@
       </c>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>73</v>
       </c>
@@ -20032,7 +20066,7 @@
       </c>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>74</v>
       </c>
@@ -20041,7 +20075,7 @@
       </c>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>75</v>
       </c>
@@ -20050,7 +20084,7 @@
       </c>
       <c r="C78" s="2"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>76</v>
       </c>
@@ -20059,7 +20093,7 @@
       </c>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>77</v>
       </c>
@@ -20068,7 +20102,7 @@
       </c>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>78</v>
       </c>
@@ -20076,7 +20110,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>79</v>
       </c>
@@ -20084,7 +20118,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>80</v>
       </c>
@@ -20092,7 +20126,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>81</v>
       </c>
@@ -20100,7 +20134,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>82</v>
       </c>
@@ -20108,7 +20142,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>83</v>
       </c>

</xml_diff>